<commit_message>
Refresh RTL Code Coverage reports with newly proven waivers, and update documentation.
Signed-off-by: Bee Nee Lim <beenee.lim@dolphin.fr>
</commit_message>
<xml_diff>
--- a/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.0/CV32E40Pv2_regression_known_failure.xlsx
+++ b/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.0/CV32E40Pv2_regression_known_failure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dolphinintegrationfr.sharepoint.com/sites/PANTHER/Documents partages/General/CV32E40P/OpenHW Group/RTL_freeze_v2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{D9A4852B-3695-42F0-A79A-3DF3377B19F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B412389-67E2-4444-B266-7DF2AF74118B}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{D9A4852B-3695-42F0-A79A-3DF3377B19F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{754B0E9F-0531-43CB-BD06-107905568D99}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="34815" yWindow="3765" windowWidth="14160" windowHeight="8010" xr2:uid="{558A017A-CB89-4642-8489-5B32B3FCA49A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{558A017A-CB89-4642-8489-5B32B3FCA49A}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_known_issue" sheetId="1" r:id="rId1"/>
@@ -36,37 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Random</t>
   </si>
   <si>
-    <t>corev_rand_interrupt_nested</t>
-  </si>
-  <si>
-    <t>Simulation error due to Interrupt routine handler is playing with mstatus.fs, leaving it at OFF state when exited. This corrupts the global setting made by TEST_CFG=floating_pt_instr_en.
-Status: Pending fix</t>
-  </si>
-  <si>
-    <t>corev_rand_pulp_hwloop_test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">illegal DUT response to a set of asynchronous net changes
-mismatches on dcrs registers
-mismatches on these instr(s) -&gt; bnez,  cv.srl.sc.h, wfi, remu, lw
-</t>
-  </si>
-  <si>
-    <t>corev_rand_debug, corev_rand_interrupt_debug, corev_rand_pulp_hwloop_debug, corev_rand_pulp_instr_debug, corev_rand_interrupt_debug, corev_rand_debug_ebreak, corev_rand_pulp_hwloop_count_range_test</t>
-  </si>
-  <si>
-    <t>Simulation error due to ebreak and haltreq at same time and ISS model has different priority in serving compare to core.
-Status: Pending updates from Imperas ISS model to have same behaviour as core.</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Example error message(s)</t>
   </si>
   <si>
@@ -88,21 +62,33 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Imperas</t>
-  </si>
-  <si>
-    <t>verif</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t xml:space="preserve">Open (80% fixed) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Build error due to offset between hwloop0_end_stream1_id0 label and cv.endi instruction can not fit in 12 bits.
-Status: Pending fix but in lower priority because is seed related and very rare to occur. 
-</t>
+    <t>corev_directed_for_hwloop_covg_test</t>
+  </si>
+  <si>
+    <t>test_program/corev_directed_for_hwloop_covg_test_550986902.S:826:(.text+0xbb4): relocation truncated to fit: R_RISCV_CVPCREL_UI12 against `hwloop1_end_stream1_id0'</t>
+  </si>
+  <si>
+    <t>Open (no fix)</t>
+  </si>
+  <si>
+    <t>corev_rand_fp_instr_debug_test_with_int_debug_trigger_and_single_step</t>
+  </si>
+  <si>
+    <t># (IDV) Instruction executed prior to mismatch '0x1a110d1e(debug_end+48): 02c3a587 flw     f11,44(x7)'</t>
+  </si>
+  <si>
+    <t>Test generation corner case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instruction number in HWLOOP body exceeding maximum number of instruction when using immediate version of HWLOOP instructions (cv.counti, cv.setupi).
+This issue seen rarely, maybe 1 out of 2~3 regressions. Too risky to fix it now as it might affect other tests. </t>
+  </si>
+  <si>
+    <t>Load in Virtual Peripheral area
+x7 set to 0x0fffffce and going to 0x10000002 with some load address offset</t>
   </si>
 </sst>
 </file>
@@ -172,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -180,20 +166,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -211,10 +191,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,139 +510,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2801443F-571E-4F33-B8FF-9C74110C36E8}">
-  <dimension ref="B2:I7"/>
+  <dimension ref="B2:I4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="84.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="84.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="60" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="6" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="G3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="2:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -674,15 +610,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="254d2fc45a10493323dcacd51be5aaf4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="003ab9e0b5c5bed7880e662758cd0922" ns2:_="" ns3:_="">
     <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
@@ -931,6 +858,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -943,14 +879,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501FC33E-FA44-4510-8B0D-EC26BDB2B6BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2873F165-068F-468F-A91D-ECB4A96B4E48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -969,6 +897,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501FC33E-FA44-4510-8B0D-EC26BDB2B6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{645BCCA5-78F8-4F1E-B54F-0CA30D08BEEE}">
   <ds:schemaRefs>

</xml_diff>